<commit_message>
perubahan modul list barang
</commit_message>
<xml_diff>
--- a/public/format/barang.xlsx
+++ b/public/format/barang.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noval\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cwa_scmfix\public\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEF3C7C-78D2-449C-9730-8DF523E6B2E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Noval</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nama</t>
   </si>
@@ -99,12 +100,15 @@
   </si>
   <si>
     <t>kode</t>
+  </si>
+  <si>
+    <t>kemasan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,11 +432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +445,7 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -455,6 +459,9 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>